<commit_message>
Get the last updates wihtin solution Migrate solution to Studio 2021
</commit_message>
<xml_diff>
--- a/SDLMTCloud.Languages.Provider/Resources/DefaultMTLanguageCodes.xlsx
+++ b/SDLMTCloud.Languages.Provider/Resources/DefaultMTLanguageCodes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSTS\Sdl-Community\Sdl.MTCloud.Languages.Provider\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSTS\Sdl-Community\SDLMTCloud.Languages.Provider\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4592,8 +4592,8 @@
   <dimension ref="A1:F632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B210" sqref="B210"/>
+      <pane ySplit="1" topLeftCell="A527" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C548" sqref="C548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>